<commit_message>
Automatische test-sync: 2025-08-30 18:34:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-30.xlsx
+++ b/logs/mail_log_2025-08-30.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -725,8 +725,50 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Opvolging bestelling</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Inkoop / Bestellingen</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-08-30 18:34:31</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2">
+  <conditionalFormatting sqref="D2:D3">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -746,7 +788,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2">
+  <conditionalFormatting sqref="G2:G3">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -754,17 +796,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2">
+  <conditionalFormatting sqref="H2:H3">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2">
+  <conditionalFormatting sqref="I2:I3">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2">
+  <conditionalFormatting sqref="J2:J3">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -806,7 +848,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-30 18:39:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-30.xlsx
+++ b/logs/mail_log_2025-08-30.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2</f>
+              <f>'Dashboard'!$A$2:$A$3</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2</f>
+              <f>'Dashboard'!$B$2:$B$3</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -767,8 +767,50 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Afspraak demo</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-08-30 18:39:20</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D3">
+  <conditionalFormatting sqref="D2:D4">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -788,7 +830,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G3">
+  <conditionalFormatting sqref="G2:G4">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -796,17 +838,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H3">
+  <conditionalFormatting sqref="H2:H4">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I3">
+  <conditionalFormatting sqref="I2:I4">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J3">
+  <conditionalFormatting sqref="J2:J4">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -821,7 +863,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -851,6 +893,16 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-30 19:03:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-30.xlsx
+++ b/logs/mail_log_2025-08-30.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$3</f>
+              <f>'Dashboard'!$A$2:$A$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$3</f>
+              <f>'Dashboard'!$B$2:$B$4</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -809,8 +809,50 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Klacht levering</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Klacht / Probleem</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2025-08-30 19:03:01</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D4">
+  <conditionalFormatting sqref="D2:D5">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -830,7 +872,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G4">
+  <conditionalFormatting sqref="G2:G5">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -838,17 +880,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H4">
+  <conditionalFormatting sqref="H2:H5">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I4">
+  <conditionalFormatting sqref="I2:I5">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J4">
+  <conditionalFormatting sqref="J2:J5">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -863,7 +905,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -903,6 +945,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Klacht / Probleem</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-30 19:05:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-30.xlsx
+++ b/logs/mail_log_2025-08-30.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -851,8 +851,50 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Opvolging klacht</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Klacht / Probleem</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2025-08-30 19:05:06</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D5">
+  <conditionalFormatting sqref="D2:D6">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -872,7 +914,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G5">
+  <conditionalFormatting sqref="G2:G6">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -880,17 +922,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H5">
+  <conditionalFormatting sqref="H2:H6">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I5">
+  <conditionalFormatting sqref="I2:I6">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J5">
+  <conditionalFormatting sqref="J2:J6">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -938,17 +980,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Planning / Afspraak</t>
+          <t>Klacht / Probleem</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Klacht / Probleem</t>
+          <t>Planning / Afspraak</t>
         </is>
       </c>
       <c r="B4" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-30 19:24:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-30.xlsx
+++ b/logs/mail_log_2025-08-30.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$4</f>
+              <f>'Dashboard'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$4</f>
+              <f>'Dashboard'!$B$2:$B$5</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -893,8 +893,50 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Bel klant</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Klantenservice / Contact</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2025-08-30 19:24:30</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D6">
+  <conditionalFormatting sqref="D2:D7">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -914,7 +956,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G6">
+  <conditionalFormatting sqref="G2:G7">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -922,17 +964,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H6">
+  <conditionalFormatting sqref="H2:H7">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I6">
+  <conditionalFormatting sqref="I2:I7">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J6">
+  <conditionalFormatting sqref="J2:J7">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -947,7 +989,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -997,6 +1039,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Klantenservice / Contact</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-30 19:26:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-30.xlsx
+++ b/logs/mail_log_2025-08-30.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -935,8 +935,50 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Opvolging contact</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Klantenservice / Contact</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2025-08-30 19:26:33</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D7">
+  <conditionalFormatting sqref="D2:D8">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -956,7 +998,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G7">
+  <conditionalFormatting sqref="G2:G8">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -964,17 +1006,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H7">
+  <conditionalFormatting sqref="H2:H8">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I7">
+  <conditionalFormatting sqref="I2:I8">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J7">
+  <conditionalFormatting sqref="J2:J8">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1032,17 +1074,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Planning / Afspraak</t>
+          <t>Klantenservice / Contact</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Klantenservice / Contact</t>
+          <t>Planning / Afspraak</t>
         </is>
       </c>
       <c r="B5" t="n">

</xml_diff>